<commit_message>
budzets un izdevumi (ieskats)
</commit_message>
<xml_diff>
--- a/budzeta_limitu_kopsavilkums.xlsx
+++ b/budzeta_limitu_kopsavilkums.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>150</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>150</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43.5</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>43.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40.5</v>
+        <v>40</v>
       </c>
       <c r="C7" t="n">
-        <v>40.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,7 +646,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-09 13:29:14</t>
+          <t>2025-05-09 18:55:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>167.9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-09 13:29:59</t>
+          <t>2025-05-09 18:55:11</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -670,13 +670,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>15.6</v>
+        <v>23.32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-05-09 13:30:49</t>
+          <t>2025-05-09 18:55:39</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -685,67 +685,322 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>153.4</v>
+        <v>111.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:31:29</t>
+          <t>2025-05-09 18:55:45</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>apģērbs</t>
+          <t>hobiji</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10.32</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-09 13:31:56</t>
+          <t>2025-05-09 18:55:48</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>higēnas preces</t>
+          <t>mājdzīvnieki</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:16</t>
+          <t>2025-05-09 18:55:56</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>medicīniskie izdevumi</t>
+          <t>apģērbs</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>13.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:33</t>
+          <t>2025-05-09 18:55:58</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>higēnas preces</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>medicīniskie izdevumi</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:05</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>transports</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:09</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>izklaide (kino, teātris, klubs)</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>abonementi</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C12" t="n">
         <v>19.99</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>dāvanas</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:28</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>pārtika</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:30</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ēšana ārpus mājas (restorāni/fast food/kafejnīcas)</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:31</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mājas izdevumi (komunālie + īre / nekustamā īpašuma nodoklis)</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:31</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>hobiji</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:32</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mājdzīvnieki</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:32</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>apģērbs</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:33</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>higēnas preces</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:34</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>medicīniskie izdevumi</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:35</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>transports</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:36</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>izklaide (kino, teātris, klubs)</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:36</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>abonementi</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-09 18:56:37</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>dāvanas</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.daļa (japabeidz lidz galam izdevumi, jaizskata, vai  viss iet)
</commit_message>
<xml_diff>
--- a/budzeta_limitu_kopsavilkums.xlsx
+++ b/budzeta_limitu_kopsavilkums.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="C2" t="n">
-        <v>23</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23</v>
+        <v>400</v>
       </c>
       <c r="C5" t="n">
-        <v>23</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>234</v>
       </c>
       <c r="C7" t="n">
-        <v>40</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1234</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="9">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
@@ -601,10 +601,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,373 +634,8 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Kategorija</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Izdevums</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:00</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>pārtika</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:11</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ēšana ārpus mājas (restorāni/fast food/kafejnīcas)</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>23.32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:39</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mājas izdevumi (komunālie + īre / nekustamā īpašuma nodoklis)</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>111.5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:45</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>hobiji</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:48</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>mājdzīvnieki</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:56</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>apģērbs</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>13.99</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:55:58</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>higēnas preces</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:01</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>medicīniskie izdevumi</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:05</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>transports</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:09</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>izklaide (kino, teātris, klubs)</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:12</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>abonementi</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>19.99</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:14</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>dāvanas</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:28</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>pārtika</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:30</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>ēšana ārpus mājas (restorāni/fast food/kafejnīcas)</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:31</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>mājas izdevumi (komunālie + īre / nekustamā īpašuma nodoklis)</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:31</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>hobiji</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:32</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>mājdzīvnieki</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:32</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>apģērbs</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:33</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>higēnas preces</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:34</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>medicīniskie izdevumi</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:35</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>transports</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:36</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>izklaide (kino, teātris, klubs)</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:36</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>abonementi</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-05-09 18:56:37</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>dāvanas</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
+          <t>KategorijaIzdevums</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6. daļa (rediģēšanas funkcija)
</commit_message>
<xml_diff>
--- a/budzeta_limitu_kopsavilkums.xlsx
+++ b/budzeta_limitu_kopsavilkums.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="C2" t="n">
-        <v>230</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23</v>
+        <v>450</v>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>400</v>
+        <v>123</v>
       </c>
       <c r="C5" t="n">
-        <v>400</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>242</v>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>234</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>234</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1234</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>1234</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>32</v>
+        <v>200.3</v>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>200.3</v>
       </c>
     </row>
     <row r="10">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13</v>
+        <v>12.2</v>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="11">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>13</v>
+        <v>13.2</v>
       </c>
       <c r="C11" t="n">
-        <v>13</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="12">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44</v>
+        <v>1.99</v>
       </c>
       <c r="C12" t="n">
-        <v>44</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="13">
@@ -601,10 +601,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,7 +634,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>KategorijaIzdevums</t>
+          <t>Kategorija</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Izdevums</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
20.05.25 (pievienoti komentari, finala korekcijas)
</commit_message>
<xml_diff>
--- a/budzeta_limitu_kopsavilkums.xlsx
+++ b/budzeta_limitu_kopsavilkums.xlsx
@@ -435,8 +435,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>2</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Kategorija</t>
+        </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -456,10 +458,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>35.68</v>
       </c>
     </row>
     <row r="3">
@@ -469,10 +471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="4">
@@ -482,10 +484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>16.79</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -508,10 +510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>16.79</v>
       </c>
     </row>
     <row r="7">
@@ -521,10 +523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -534,10 +536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -547,10 +549,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -560,10 +562,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -573,10 +575,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -586,10 +588,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -599,10 +601,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -644,31 +646,121 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-20 10:36:03</t>
+          <t>2025-05-20 17:52:39</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>apģērbs</t>
+          <t>pārtika</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>14.32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-20 10:36:53</t>
+          <t>2025-05-20 17:52:48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pārtika</t>
+          <t>mājas izdevumi (komunālie + īre / nekustamā īpašuma nodoklis)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:52:56</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hobiji</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:53:10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ēšana ārpus mājas (restorāni/fast food/kafejnīcas)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:53:16</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dāvanas</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>11.34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:53:32</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dāvanas</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:53:42</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>medicīniskie izdevumi</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-20 17:53:53</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mājdzīvnieki</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>13.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>